<commit_message>
fix import error and update CSVs
</commit_message>
<xml_diff>
--- a/W40K-HOI4 Converter.xlsx
+++ b/W40K-HOI4 Converter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/429d0bbe9bd122b3/Logiciels et Jeux/Heart of Iron IV/HOI4_Calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{30E7DDE0-7559-F044-BCCF-868894B9CFCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{30E7DDE0-7559-F044-BCCF-868894B9CFCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F158DB8-F769-8247-B4F5-97143FF819AA}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="29970" yWindow="1170" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{D4C3DD04-2F54-554F-9DFA-AF0108F6C81D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16740" activeTab="2" xr2:uid="{D4C3DD04-2F54-554F-9DFA-AF0108F6C81D}"/>
   </bookViews>
   <sheets>
     <sheet name="SA et HA" sheetId="1" r:id="rId1"/>
@@ -197,21 +197,6 @@
   </cellStyles>
   <dxfs count="21">
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -230,6 +215,21 @@
       </font>
       <numFmt numFmtId="164" formatCode="0.0"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
     <dxf>
       <font>
@@ -1582,7 +1582,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AC16A1AC-14A9-A741-BF9F-860BF516F5B2}" type="CELLRANGE">
+                    <a:fld id="{21866E60-5E46-724C-9C1F-E4C986876666}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -1615,8 +1615,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A6770A42-54CE-CD4F-B8F2-21D502DC4888}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{76CDEDD9-DCE4-A24F-9EFC-E5478280C122}" type="CELLRANGE">
+                      <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
                     </a:fld>
@@ -1634,6 +1634,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1648,8 +1649,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{29F85460-5841-BC4D-8167-3C7BA909233E}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{18758913-E5B3-6A41-AB9A-50C06E89C547}" type="CELLRANGE">
+                      <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
                     </a:fld>
@@ -1667,6 +1668,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1681,8 +1683,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0DC62D4A-C6D5-A646-85A9-A4DC5F88C2C1}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{1954D013-3394-C54F-82D2-13F9394DEA7C}" type="CELLRANGE">
+                      <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
                     </a:fld>
@@ -1700,6 +1702,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1714,8 +1717,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6C410983-46FC-4342-B620-500A3C7B5A58}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{7E23D6BD-E80A-9245-8260-EE4CF0C2EEE0}" type="CELLRANGE">
+                      <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
                     </a:fld>
@@ -1733,6 +1736,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1747,8 +1751,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{138B53B6-EDA3-5241-812D-6B3A044E40DF}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{6CFA5509-3416-EE45-938E-E6AAFFC28D33}" type="CELLRANGE">
+                      <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
                     </a:fld>
@@ -1766,6 +1770,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1780,8 +1785,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{00756374-ECAD-194D-A2C0-96658856E94C}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{60F2BEC2-37E3-2D40-AC86-7FFA73F14525}" type="CELLRANGE">
+                      <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
                     </a:fld>
@@ -1799,6 +1804,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1813,8 +1819,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{99F9CD0B-EA10-B448-9AA2-77814908DF7D}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{67AE82C2-3BA8-904E-80E8-61B19453B444}" type="CELLRANGE">
+                      <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
                     </a:fld>
@@ -1832,6 +1838,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1846,8 +1853,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8EAA7AAA-7468-C842-9172-7704169D8F4F}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{2F291F7A-96D9-9645-8971-D2FA706869C1}" type="CELLRANGE">
+                      <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
                     </a:fld>
@@ -1865,6 +1872,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1879,8 +1887,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E41EC8FE-A3C1-3A49-B246-4C89640B9F87}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{1C4215E8-F5C1-0C47-AE27-0CC5C249E157}" type="CELLRANGE">
+                      <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
                     </a:fld>
@@ -1898,6 +1906,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1992,34 +2001,34 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.44444444444444442</c:v>
+                  <c:v>1.6487212707001282E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>2.7182818284590449E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>4.4816890703380644E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5</c:v>
+                  <c:v>7.3890560989306506E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.25</c:v>
+                  <c:v>0.12182493960703474</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.375</c:v>
+                  <c:v>0.20085536923187669</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.0625</c:v>
+                  <c:v>0.3311545195869231</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.59375</c:v>
+                  <c:v>0.54598150033144233</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11.390625</c:v>
+                  <c:v>0.90017131300521813</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>17.0859375</c:v>
+                  <c:v>1.484131591025766</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2032,34 +2041,34 @@
                 <c15:dlblRangeCache>
                   <c:ptCount val="10"/>
                   <c:pt idx="0">
-                    <c:v>0,4</c:v>
+                    <c:v>0,0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0,7</c:v>
+                    <c:v>0,0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1,0</c:v>
+                    <c:v>0,0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1,5</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2,3</c:v>
+                    <c:v>0,1</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>3,4</c:v>
+                    <c:v>0,2</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>5,1</c:v>
+                    <c:v>0,3</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>7,6</c:v>
+                    <c:v>0,5</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>11,4</c:v>
+                    <c:v>0,9</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>17,1</c:v>
+                    <c:v>1,5</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -4246,13 +4255,15 @@
   <autoFilter ref="A2:H12" xr:uid="{4B6B9677-3CC6-274A-B76C-365663A705CB}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{9EB72AAB-E345-6949-90B2-EF5C02C4735E}" name="E / HP"/>
-    <tableColumn id="9" xr3:uid="{77A34681-2086-A749-A721-27F7398FABEB}" name="-" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{8820C6AE-5E1E-2046-9B4B-88D33201E54E}" name="Colonne1" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{0528867D-BFAB-D841-8103-23F69C8C64F2}" name="Colonne2" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{83EF4AD6-487F-8A4F-AAF2-B0E660AE2C9C}" name="Colonne3" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{37F7CDA7-B8DA-CC49-A998-E1429D5E1F19}" name="Colonne4" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{16B04AFD-D425-7C49-8211-BA56537C0D1F}" name="Colonne5" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{F074B7DE-CDF5-8D4E-A044-1E1D25EBC904}" name="Colonne6" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{77A34681-2086-A749-A721-27F7398FABEB}" name="-" dataDxfId="0">
+      <calculatedColumnFormula>EXP(A3/2) /100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{8820C6AE-5E1E-2046-9B4B-88D33201E54E}" name="Colonne1" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{0528867D-BFAB-D841-8103-23F69C8C64F2}" name="Colonne2" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{83EF4AD6-487F-8A4F-AAF2-B0E660AE2C9C}" name="Colonne3" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{37F7CDA7-B8DA-CC49-A998-E1429D5E1F19}" name="Colonne4" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{16B04AFD-D425-7C49-8211-BA56537C0D1F}" name="Colonne5" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{F074B7DE-CDF5-8D4E-A044-1E1D25EBC904}" name="Colonne6" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4561,12 +4572,12 @@
       <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.875" style="2"/>
+    <col min="2" max="2" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
@@ -4586,7 +4597,7 @@
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4636,7 +4647,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4698,7 +4709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4762,7 +4773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4826,7 +4837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4890,7 +4901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4953,7 +4964,7 @@
         <v>3.8201625000000012</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -5017,7 +5028,7 @@
         <v>5.0808161250000001</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -5081,7 +5092,7 @@
         <v>6.7574854462500031</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -5145,7 +5156,7 @@
         <v>8.9874556435125008</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -5209,7 +5220,7 @@
         <v>11.953316005871628</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -5351,16 +5362,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F97B4F1-F554-1842-9830-8AFE983B6720}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.125" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -5377,7 +5388,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -5388,7 +5399,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -5399,12 +5410,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -5415,7 +5426,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -5426,7 +5437,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -5437,7 +5448,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -5452,7 +5463,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -5463,7 +5474,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -5471,7 +5482,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -5479,7 +5490,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -5523,16 +5534,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2399AF44-C230-AD45-8055-01F99E7221A4}">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView zoomScale="107" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.875" style="2"/>
+    <col min="2" max="2" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
@@ -5550,7 +5561,7 @@
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -5577,13 +5588,13 @@
       </c>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="3">
-        <f>B4/1.5</f>
-        <v>0.44444444444444442</v>
+        <f t="shared" ref="B3:B12" si="0">EXP(A3/2) /100</f>
+        <v>1.6487212707001282E-2</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -5599,13 +5610,13 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" s="3">
-        <f>B5/1.5</f>
-        <v>0.66666666666666663</v>
+        <f t="shared" si="0"/>
+        <v>2.7182818284590449E-2</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -5621,12 +5632,13 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" s="3">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>4.4816890703380644E-2</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -5642,13 +5654,13 @@
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" s="3">
-        <f t="shared" ref="B6:B12" si="0">B5*1.5</f>
-        <v>1.5</v>
+        <f t="shared" si="0"/>
+        <v>7.3890560989306506E-2</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -5664,13 +5676,13 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" s="3">
         <f t="shared" si="0"/>
-        <v>2.25</v>
+        <v>0.12182493960703474</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -5686,13 +5698,13 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" s="3">
         <f t="shared" si="0"/>
-        <v>3.375</v>
+        <v>0.20085536923187669</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -5708,13 +5720,13 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" s="3">
         <f t="shared" si="0"/>
-        <v>5.0625</v>
+        <v>0.3311545195869231</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -5730,13 +5742,13 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" s="3">
         <f t="shared" si="0"/>
-        <v>7.59375</v>
+        <v>0.54598150033144233</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -5752,13 +5764,13 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" s="3">
         <f t="shared" si="0"/>
-        <v>11.390625</v>
+        <v>0.90017131300521813</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -5774,13 +5786,13 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" s="3">
         <f t="shared" si="0"/>
-        <v>17.0859375</v>
+        <v>1.484131591025766</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>

</xml_diff>

<commit_message>
MAJOR - BRK and DEF
- split SA HA and BRK DEF bonus functions for weapons
- Update CSV
- fix tank generation
- added Company bonuses
- reset DEF and BRK calculation regards F and PA to 1 all the time
- added SP artillery and the Destroyer in function as vehicle weapons
</commit_message>
<xml_diff>
--- a/W40K-HOI4 Converter.xlsx
+++ b/W40K-HOI4 Converter.xlsx
@@ -197,6 +197,21 @@
   </cellStyles>
   <dxfs count="21">
     <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -215,21 +230,6 @@
       </font>
       <numFmt numFmtId="164" formatCode="0.0"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
     <dxf>
       <font>
@@ -1615,7 +1615,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{76CDEDD9-DCE4-A24F-9EFC-E5478280C122}" type="CELLRANGE">
+                    <a:fld id="{26C9ABEB-47E2-D742-A5D9-7FBDCE656EB5}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -1649,7 +1649,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{18758913-E5B3-6A41-AB9A-50C06E89C547}" type="CELLRANGE">
+                    <a:fld id="{A065FD2B-BD2D-C14B-B9D6-805C7E3D68E3}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -1683,7 +1683,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1954D013-3394-C54F-82D2-13F9394DEA7C}" type="CELLRANGE">
+                    <a:fld id="{D11FC217-0B6F-AE47-9594-3D69BA26D4A2}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -1717,7 +1717,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7E23D6BD-E80A-9245-8260-EE4CF0C2EEE0}" type="CELLRANGE">
+                    <a:fld id="{6079167F-7912-D64B-ADCE-DCC9CBC9E2DE}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -1751,7 +1751,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6CFA5509-3416-EE45-938E-E6AAFFC28D33}" type="CELLRANGE">
+                    <a:fld id="{9E19C1A2-B182-7644-A6AA-F1C75727195B}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -1785,7 +1785,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{60F2BEC2-37E3-2D40-AC86-7FFA73F14525}" type="CELLRANGE">
+                    <a:fld id="{1F56B3A3-78B2-B64D-9BDD-5CB9B4D3426A}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -1819,7 +1819,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{67AE82C2-3BA8-904E-80E8-61B19453B444}" type="CELLRANGE">
+                    <a:fld id="{3A84342B-4F9F-3D48-A7B7-ED660A4FECA2}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -1853,7 +1853,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2F291F7A-96D9-9645-8971-D2FA706869C1}" type="CELLRANGE">
+                    <a:fld id="{2943E72A-3A11-9A44-BA8B-F9AB1F171F9D}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -1887,7 +1887,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1C4215E8-F5C1-0C47-AE27-0CC5C249E157}" type="CELLRANGE">
+                    <a:fld id="{EE4B413F-E95D-2840-8B75-F8973FD05B2B}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -4255,15 +4255,15 @@
   <autoFilter ref="A2:H12" xr:uid="{4B6B9677-3CC6-274A-B76C-365663A705CB}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{9EB72AAB-E345-6949-90B2-EF5C02C4735E}" name="E / HP"/>
-    <tableColumn id="9" xr3:uid="{77A34681-2086-A749-A721-27F7398FABEB}" name="-" dataDxfId="0">
+    <tableColumn id="9" xr3:uid="{77A34681-2086-A749-A721-27F7398FABEB}" name="-" dataDxfId="6">
       <calculatedColumnFormula>EXP(A3/2) /100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{8820C6AE-5E1E-2046-9B4B-88D33201E54E}" name="Colonne1" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{0528867D-BFAB-D841-8103-23F69C8C64F2}" name="Colonne2" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{83EF4AD6-487F-8A4F-AAF2-B0E660AE2C9C}" name="Colonne3" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{37F7CDA7-B8DA-CC49-A998-E1429D5E1F19}" name="Colonne4" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{16B04AFD-D425-7C49-8211-BA56537C0D1F}" name="Colonne5" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{F074B7DE-CDF5-8D4E-A044-1E1D25EBC904}" name="Colonne6" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{8820C6AE-5E1E-2046-9B4B-88D33201E54E}" name="Colonne1" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{0528867D-BFAB-D841-8103-23F69C8C64F2}" name="Colonne2" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{83EF4AD6-487F-8A4F-AAF2-B0E660AE2C9C}" name="Colonne3" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{37F7CDA7-B8DA-CC49-A998-E1429D5E1F19}" name="Colonne4" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{16B04AFD-D425-7C49-8211-BA56537C0D1F}" name="Colonne5" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{F074B7DE-CDF5-8D4E-A044-1E1D25EBC904}" name="Colonne6" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5535,7 +5535,7 @@
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>